<commit_message>
Add more historical data.
</commit_message>
<xml_diff>
--- a/real_world/brittany_tokai_villas/2022_2023/ReserveFundBudget.xlsx
+++ b/real_world/brittany_tokai_villas/2022_2023/ReserveFundBudget.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" state="visible" r:id="rId2"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="145">
   <si>
     <t xml:space="preserve">ReserveFundBudget</t>
   </si>
@@ -464,19 +464,22 @@
     <t xml:space="preserve">Budget Summary</t>
   </si>
   <si>
-    <t xml:space="preserve">This worksheet summarizes the changes in the budget and</t>
+    <t xml:space="preserve">This worksheet summarizes the administrative and reserve fund budgets, </t>
   </si>
   <si>
-    <t xml:space="preserve">reserves for the current year over the previous financial</t>
+    <t xml:space="preserve">the health of the reserve fund and the financial pressure that the ten</t>
   </si>
   <si>
-    <t xml:space="preserve">year.</t>
+    <t xml:space="preserve">year plan imposes on the reserve fund.</t>
   </si>
   <si>
     <t xml:space="preserve">Administrative budget</t>
   </si>
   <si>
     <t xml:space="preserve">Reserve fund budget</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum reserve budget [per PMR22(2)]</t>
   </si>
   <si>
     <t xml:space="preserve">Total budget</t>
@@ -497,25 +500,13 @@
     <t xml:space="preserve">Initial reserves</t>
   </si>
   <si>
-    <t xml:space="preserve">Recommended initial reserves</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actual versus recommended difference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actual versus recommended difference (%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Projected final reserves at year end</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Recommended final reserves</t>
+    <t xml:space="preserve">Projected final reserves</t>
   </si>
   <si>
     <t xml:space="preserve">Percentage change in reserves</t>
   </si>
   <si>
-    <t xml:space="preserve">Reserves in months</t>
+    <t xml:space="preserve">Projected final reserves in months</t>
   </si>
   <si>
     <t xml:space="preserve">Ten Year Plan Summary</t>
@@ -1003,11 +994,11 @@
   </sheetPr>
   <dimension ref="A1:A27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="80.03"/>
   </cols>
@@ -1153,7 +1144,7 @@
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="51.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.72"/>
@@ -1329,7 +1320,7 @@
       <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.59"/>
@@ -5248,10 +5239,10 @@
   <dimension ref="A1:AY94"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
@@ -17867,7 +17858,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="true" objects="true" scenarios="true"/>
   <mergeCells count="15">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A2:E2"/>
@@ -17906,7 +17896,7 @@
       <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="53.35"/>
   </cols>
@@ -18665,15 +18655,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="46.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.95"/>
   </cols>
   <sheetData>
@@ -18709,36 +18699,41 @@
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="47" t="s">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="47" t="s">
         <v>124</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" s="32" t="n">
+        <f aca="false">'Current Financials'!B15</f>
+        <v>1194840</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="41" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B9" s="32" t="n">
-        <f aca="false">'Current Financials'!B15</f>
-        <v>1194840</v>
+        <f aca="false">'Planning and Projections'!B22</f>
+        <v>349815.32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="41" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B10" s="32" t="n">
-        <f aca="false">'Planning and Projections'!B22</f>
-        <v>349815.32</v>
+        <f aca="false">'Current Year Planner'!E15</f>
+        <v>353204.332549415</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="41" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B11" s="32" t="n">
         <f aca="false">'Planning and Projections'!B21</f>
@@ -18747,16 +18742,16 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="41" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B12" s="48" t="n">
-        <f aca="false">B10/B11</f>
+        <f aca="false">B9/B11</f>
         <v>0.226468206512246</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="41" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B13" s="32" t="n">
         <f aca="false">'Current Financials'!B14</f>
@@ -18765,7 +18760,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="41" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B14" s="48" t="n">
         <f aca="false">B11/'Current Financials'!B14-1</f>
@@ -18778,13 +18773,13 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="47" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B16" s="48"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="41" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B17" s="32" t="n">
         <f aca="false">'Planning and Projections'!B18</f>
@@ -18793,131 +18788,69 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="41" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B18" s="32" t="n">
-        <f aca="false">'Current Year Planner'!E13</f>
-        <v>2083550</v>
+        <f aca="false">'Planning and Projections'!B26</f>
+        <v>1661535.6365</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="B19" s="32" t="n">
-        <f aca="false">B17-B18</f>
-        <v>-119095</v>
+        <v>138</v>
+      </c>
+      <c r="B19" s="33" t="n">
+        <f aca="false">(B18-B17)/B17</f>
+        <v>-0.154200204891433</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="41" t="s">
-        <v>138</v>
-      </c>
-      <c r="B20" s="33" t="n">
-        <f aca="false">(B17-B18)/B18</f>
-        <v>-0.0571596553958388</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="41"/>
-      <c r="B21" s="32"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="41" t="s">
         <v>139</v>
       </c>
-      <c r="B22" s="32" t="n">
-        <f aca="false">'Planning and Projections'!B26</f>
-        <v>1661535.6365</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="41" t="s">
-        <v>140</v>
-      </c>
-      <c r="B23" s="32" t="n">
-        <f aca="false">'Current Year Planner'!E19</f>
-        <v>1664967.01170628</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="41" t="s">
-        <v>137</v>
-      </c>
-      <c r="B24" s="32" t="n">
-        <f aca="false">B22-B23</f>
-        <v>-3431.37520628213</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="41" t="s">
-        <v>138</v>
-      </c>
-      <c r="B25" s="33" t="n">
-        <f aca="false">(B22-B23)/B23</f>
-        <v>-0.00206092684248777</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="41"/>
-      <c r="B26" s="32"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="41" t="s">
-        <v>141</v>
-      </c>
-      <c r="B27" s="33" t="n">
-        <f aca="false">(B22-B17)/B17</f>
-        <v>-0.154200204891433</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="41" t="s">
-        <v>142</v>
-      </c>
-      <c r="B28" s="49" t="n">
+      <c r="B20" s="49" t="n">
         <f aca="false">'Planning and Projections'!B27</f>
         <v>16.6871109420508</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="47" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>144</v>
-      </c>
-      <c r="B31" s="50" t="n">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="47" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" s="50" t="n">
         <f aca="false">'Ten Year Plan'!$Q$89</f>
         <v>5681000</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="B32" s="48" t="n">
-        <f aca="false">$B$17/$B$31</f>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B24" s="48" t="n">
+        <f aca="false">$B$17/$B$23</f>
         <v>0.345793874317902</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="B33" s="50" t="n">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B25" s="50" t="n">
         <f aca="false">'Ten Year Plan'!$Q$88</f>
         <v>6941298.38673845</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="B34" s="48" t="n">
-        <f aca="false">$B$17/$B$33</f>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B26" s="48" t="n">
+        <f aca="false">$B$17/$B$25</f>
         <v>0.283009732552796</v>
       </c>
     </row>

</xml_diff>